<commit_message>
volume control fix and battery level checker
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Todos</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Mention HolaDeviceData class in Hola App Document</t>
+  </si>
+  <si>
+    <t>Battery level check with led bar</t>
+  </si>
+  <si>
+    <t>Improve streaming performance</t>
+  </si>
+  <si>
+    <t>App support for intercom moving to new WiFi network</t>
   </si>
 </sst>
 </file>
@@ -529,10 +538,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -900,6 +909,30 @@
       </c>
       <c r="C43" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multiple fixes and improvements. See description
- Added COMM_START/STOP+ACK messages
- Incoming communication (COMM_START) enables recording and ratetuning.
- Further stablized buddy listening FSM
- Added sequence number to voice_data message to track lost
communication and stuff circular buffer.
- Tweaked rate tuning params.
- Intercom_Outgoing API and FSM to allow multiple requesters to enable
recording.
- Using codec patch 2.01
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -19,6 +19,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>Todos</t>
   </si>
@@ -202,6 +203,54 @@
   </si>
   <si>
     <t>App support for intercom moving to new WiFi network</t>
+  </si>
+  <si>
+    <t>LEDs keep flashing after reset</t>
+  </si>
+  <si>
+    <t>Stabilize not listen -&gt; listen FSM</t>
+  </si>
+  <si>
+    <t>Stabilize startup / WiFi/ cloud connection</t>
+  </si>
+  <si>
+    <t>RateTuning</t>
+  </si>
+  <si>
+    <t>Activate recording when incoming data</t>
+  </si>
+  <si>
+    <t>VU meter</t>
+  </si>
+  <si>
+    <t>Add FSM diagrams</t>
+  </si>
+  <si>
+    <t>Add WiFi signal strength to cloud API and app</t>
+  </si>
+  <si>
+    <t>Used 5 band equalizer</t>
+  </si>
+  <si>
+    <t>Install stronger speaker</t>
+  </si>
+  <si>
+    <t>Only send EchoReq as keep-alive when no incoming comm.</t>
+  </si>
+  <si>
+    <t>Use exponential back-off for EchoReq</t>
+  </si>
+  <si>
+    <t>Add permission flag to cloud API to allow recording enable by remote</t>
+  </si>
+  <si>
+    <t>Add support for / experiment with ECB mode encryption</t>
+  </si>
+  <si>
+    <t>Experiment with ADPCM 16MHz mode</t>
+  </si>
+  <si>
+    <t>Root cause voice_data message loss in duplex mode</t>
   </si>
 </sst>
 </file>
@@ -538,15 +587,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" customWidth="1"/>
     <col min="3" max="3" width="24.109375" customWidth="1"/>
     <col min="4" max="4" width="40.77734375" style="3" customWidth="1"/>
   </cols>
@@ -935,6 +984,134 @@
         <v>9</v>
       </c>
     </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added FSMs to documentation
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -590,7 +590,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,7 +1037,7 @@
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added LevelChecker and WifiLevelChecker
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -589,8 +589,8 @@
   </sheetPr>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +1045,7 @@
         <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bugfixed battery and wifi level on Cloud API
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
   <si>
     <t>Todos</t>
   </si>
@@ -251,6 +250,12 @@
   </si>
   <si>
     <t>Root cause voice_data message loss in duplex mode</t>
+  </si>
+  <si>
+    <t>Add percentage widgets for battery and wifi level in app</t>
+  </si>
+  <si>
+    <t>Sync app to latest SDK</t>
   </si>
 </sst>
 </file>
@@ -587,10 +592,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,6 +1117,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
External Antenna selected and buddy LED blinking when comm. started
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>Todos</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Sync app to latest SDK</t>
+  </si>
+  <si>
+    <t>Using LED blink instead</t>
   </si>
 </sst>
 </file>
@@ -594,8 +597,8 @@
   </sheetPr>
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +613,7 @@
         <v>44</v>
       </c>
       <c r="C1" s="2">
-        <v>43068</v>
+        <v>43119</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -675,7 +678,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,7 +981,7 @@
         <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -1005,7 +1008,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>60</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>61</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>62</v>
       </c>
@@ -1029,15 +1032,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>64</v>
       </c>
@@ -1045,15 +1051,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>66</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>67</v>
       </c>
@@ -1069,7 +1075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>68</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>69</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>70</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>71</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>72</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>73</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>74</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Response communication should stop when incoming stops
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -610,7 +610,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1172,7 +1172,7 @@
         <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Bugfix for voice_data message corruption + added decoded message prints
En/Decryption currently disabled
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$D$35</definedName>
@@ -249,9 +250,6 @@
     <t>Experiment with ADPCM 16MHz mode</t>
   </si>
   <si>
-    <t>Root cause voice_data message loss in duplex mode</t>
-  </si>
-  <si>
     <t>Add percentage widgets for battery and wifi level in app</t>
   </si>
   <si>
@@ -271,6 +269,9 @@
   </si>
   <si>
     <t>rateTuning is too slow and goes too high and lowe</t>
+  </si>
+  <si>
+    <t>Root cause voice_data message loss and corruption in duplex mode</t>
   </si>
 </sst>
 </file>
@@ -610,7 +611,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,7 +1053,7 @@
         <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
@@ -1129,15 +1130,15 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
         <v>45</v>
@@ -1145,7 +1146,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -1153,7 +1154,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -1161,7 +1162,7 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
         <v>45</v>
@@ -1169,7 +1170,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C67" t="s">
         <v>45</v>
@@ -1177,7 +1178,7 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
         <v>45</v>
@@ -1188,4 +1189,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>166</v>
+      </c>
+      <c r="B1">
+        <v>0.5</v>
+      </c>
+      <c r="C1">
+        <f>A1*B1</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C9" si="0">A2*B2</f>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>555</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>277.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>555</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>277.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>150</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>13500</f>
+        <v>13500</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <f>7000*B9</f>
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Enabled Equalizer in codec
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>Todos</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Add WiFi signal strength to cloud API and app</t>
   </si>
   <si>
-    <t>Used 5 band equalizer</t>
-  </si>
-  <si>
     <t>Install stronger speaker</t>
   </si>
   <si>
@@ -272,6 +269,15 @@
   </si>
   <si>
     <t>Root cause voice_data message loss and corruption in duplex mode</t>
+  </si>
+  <si>
+    <t>Implement voice data retransmission protocol</t>
+  </si>
+  <si>
+    <t>Use 5 band equalizer</t>
+  </si>
+  <si>
+    <t>Bug: sometimes msg comm goes haywire after speech</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +632,7 @@
         <v>44</v>
       </c>
       <c r="C1" s="2">
-        <v>43119</v>
+        <v>43132</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,7 +909,7 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -1053,7 +1059,7 @@
         <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
@@ -1074,31 +1080,31 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
@@ -1106,7 +1112,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -1114,7 +1120,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
         <v>45</v>
@@ -1122,7 +1128,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1130,15 +1136,15 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
         <v>45</v>
@@ -1146,7 +1152,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s">
         <v>9</v>
@@ -1154,7 +1160,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -1162,7 +1168,7 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s">
         <v>45</v>
@@ -1170,7 +1176,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
         <v>45</v>
@@ -1178,10 +1184,26 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C68" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced echo mechanism with simplex keep_alive
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>Todos</t>
   </si>
@@ -278,6 +278,15 @@
   </si>
   <si>
     <t>Bug: sometimes msg comm goes haywire after speech</t>
+  </si>
+  <si>
+    <t>Add SW power down</t>
+  </si>
+  <si>
+    <t>Redo server side design diagram in draw.io</t>
+  </si>
+  <si>
+    <t>Replaced by simplex keep alive mechanism</t>
   </si>
 </sst>
 </file>
@@ -614,10 +623,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1099,7 +1108,10 @@
         <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
@@ -1203,6 +1215,22 @@
         <v>82</v>
       </c>
       <c r="C70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
multiple buddy setup fixes and debug features server side
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="93">
   <si>
     <t>Todos</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Against Android policy</t>
   </si>
   <si>
-    <t>build 3rd setup, test</t>
-  </si>
-  <si>
     <t>Mention HolaDeviceData class in Hola App Document</t>
   </si>
   <si>
@@ -287,6 +284,30 @@
   </si>
   <si>
     <t>Replaced by simplex keep alive mechanism</t>
+  </si>
+  <si>
+    <t>Using yuml instead</t>
+  </si>
+  <si>
+    <t>Add button to enter setup mode</t>
+  </si>
+  <si>
+    <t>Scalable server architecture</t>
+  </si>
+  <si>
+    <t>Buddy config in app takes too long</t>
+  </si>
+  <si>
+    <t>Intercom gets stuck in UDP can't send state</t>
+  </si>
+  <si>
+    <t>Volume Control not working well</t>
+  </si>
+  <si>
+    <t>Hissing, crackling, high pitch noise come from speakers in rest</t>
+  </si>
+  <si>
+    <t>Intercom2 speaker does not work</t>
   </si>
 </sst>
 </file>
@@ -623,10 +644,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +662,7 @@
         <v>44</v>
       </c>
       <c r="C1" s="2">
-        <v>43132</v>
+        <v>43143</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -690,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -899,10 +920,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -990,7 +1008,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
@@ -998,7 +1016,7 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -1006,7 +1024,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1014,7 +1032,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1022,7 +1040,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
         <v>9</v>
@@ -1030,7 +1048,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
@@ -1038,7 +1056,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1046,7 +1064,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
         <v>45</v>
@@ -1054,7 +1072,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
         <v>45</v>
@@ -1062,18 +1080,18 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
         <v>45</v>
@@ -1081,7 +1099,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
         <v>45</v>
@@ -1089,7 +1107,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
         <v>45</v>
@@ -1097,34 +1115,34 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -1132,7 +1150,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
         <v>45</v>
@@ -1140,15 +1158,15 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
         <v>45</v>
@@ -1156,7 +1174,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
         <v>45</v>
@@ -1164,73 +1182,132 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>76</v>
       </c>
-      <c r="C66" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
         <v>77</v>
       </c>
-      <c r="C67" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>78</v>
-      </c>
       <c r="C68" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>82</v>
       </c>
-      <c r="C70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>83</v>
       </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
       <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Audio Amp shutdown function.
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
   <si>
     <t>Todos</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Remember device names in Hola App when they are offine</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Against Android policy</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>Intercom2 speaker does not work</t>
+  </si>
+  <si>
+    <t>Audio Amp shuts down when not in use</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +912,10 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -995,7 +998,7 @@
         <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
@@ -1003,28 +1006,28 @@
         <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1032,7 +1035,7 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
@@ -1040,15 +1043,15 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
@@ -1056,7 +1059,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
         <v>9</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
         <v>45</v>
@@ -1072,7 +1075,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
         <v>45</v>
@@ -1080,18 +1083,18 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" t="s">
         <v>45</v>
@@ -1099,7 +1102,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
         <v>45</v>
@@ -1107,7 +1110,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
         <v>45</v>
@@ -1115,7 +1118,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
         <v>45</v>
@@ -1123,18 +1126,18 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -1142,7 +1145,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
@@ -1150,7 +1153,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C60" t="s">
         <v>45</v>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
         <v>45</v>
@@ -1166,7 +1169,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
         <v>45</v>
@@ -1174,7 +1177,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
         <v>45</v>
@@ -1182,7 +1185,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
         <v>45</v>
@@ -1190,7 +1193,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -1198,7 +1201,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" t="s">
         <v>45</v>
@@ -1206,7 +1209,7 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C67" t="s">
         <v>45</v>
@@ -1214,7 +1217,7 @@
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C68" t="s">
         <v>45</v>
@@ -1222,7 +1225,7 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -1230,7 +1233,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
         <v>9</v>
@@ -1238,7 +1241,7 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s">
         <v>9</v>
@@ -1246,18 +1249,18 @@
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
         <v>15</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C73" t="s">
         <v>9</v>
@@ -1265,7 +1268,7 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -1273,7 +1276,7 @@
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -1281,7 +1284,7 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
         <v>9</v>
@@ -1289,7 +1292,7 @@
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
@@ -1297,18 +1300,21 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications to accomodate local builds
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
   <si>
     <t>Todos</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Audio Amp shuts down when not in use</t>
+  </si>
+  <si>
+    <t>Audio Amp and Codec Analog shut down when not in use</t>
+  </si>
+  <si>
+    <t>State device name after successful setup</t>
+  </si>
+  <si>
+    <t>Remove photon picture from device setup screen</t>
   </si>
 </sst>
 </file>
@@ -644,10 +653,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,7 +916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>34</v>
       </c>
@@ -915,7 +924,7 @@
         <v>6</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -1279,7 +1288,7 @@
         <v>87</v>
       </c>
       <c r="C75" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
@@ -1295,7 +1304,7 @@
         <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
@@ -1315,6 +1324,22 @@
       </c>
       <c r="C79" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Listening Mode support added.
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
   <si>
     <t>Todos</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>Remove photon picture from device setup screen</t>
+  </si>
+  <si>
+    <t>Pop-up on device overview screen if device is ready for setup</t>
+  </si>
+  <si>
+    <t>Intercom should continue to work even when cloud connection is lost</t>
+  </si>
+  <si>
+    <t>Remove blank screen from app</t>
   </si>
 </sst>
 </file>
@@ -653,10 +662,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,6 +1348,30 @@
         <v>95</v>
       </c>
       <c r="C81" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Robustness against loss of cloud and internet
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -16,8 +16,8 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$D$35</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
   <si>
     <t>Todos</t>
   </si>
@@ -259,9 +259,6 @@
     <t>Response communication should stop when incoming stops</t>
   </si>
   <si>
-    <t>rateTuning is too slow and goes too high and lowe</t>
-  </si>
-  <si>
     <t>Root cause voice_data message loss and corruption in duplex mode</t>
   </si>
   <si>
@@ -326,6 +323,18 @@
   </si>
   <si>
     <t>Remove blank screen from app</t>
+  </si>
+  <si>
+    <t>Move to python3</t>
+  </si>
+  <si>
+    <t>Write Hola User Guide</t>
+  </si>
+  <si>
+    <t>rateTuning is too slow and goes too high and lower</t>
+  </si>
+  <si>
+    <t>This happens when internet connection has been lost. Doesn't auto recover.</t>
   </si>
 </sst>
 </file>
@@ -662,10 +671,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,162 +682,177 @@
     <col min="2" max="2" width="59.88671875" customWidth="1"/>
     <col min="3" max="3" width="24.109375" customWidth="1"/>
     <col min="4" max="4" width="40.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2">
-        <v>43143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="2">
+        <v>43152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
@@ -836,7 +860,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -844,15 +868,15 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -860,85 +884,85 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>45</v>
@@ -946,7 +970,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
         <v>45</v>
@@ -954,15 +978,15 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -970,23 +994,23 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
         <v>45</v>
@@ -994,15 +1018,18 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
         <v>45</v>
@@ -1010,18 +1037,15 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
         <v>45</v>
@@ -1029,15 +1053,15 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
@@ -1045,31 +1069,31 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
@@ -1077,23 +1101,26 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
         <v>45</v>
@@ -1101,18 +1128,15 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
         <v>45</v>
@@ -1120,7 +1144,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
         <v>45</v>
@@ -1128,50 +1152,50 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
         <v>45</v>
@@ -1179,7 +1203,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
         <v>45</v>
@@ -1187,7 +1211,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
         <v>45</v>
@@ -1195,15 +1219,15 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s">
         <v>45</v>
@@ -1211,15 +1235,15 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
         <v>45</v>
@@ -1227,23 +1251,23 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
         <v>9</v>
@@ -1251,50 +1275,53 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C70" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
+        <v>45</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C75" t="s">
         <v>45</v>
@@ -1302,15 +1329,18 @@
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C77" t="s">
         <v>45</v>
@@ -1318,18 +1348,15 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C79" t="s">
         <v>45</v>
@@ -1337,23 +1364,23 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
@@ -1361,7 +1388,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C83" t="s">
         <v>9</v>
@@ -1369,7 +1396,7 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
LedBar flashes slowly when battery is low
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="103">
   <si>
     <t>Todos</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>This happens when internet connection has been lost. Doesn't auto recover.</t>
+  </si>
+  <si>
+    <t>Hola App is draining battery</t>
   </si>
 </sst>
 </file>
@@ -671,10 +674,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1399,6 +1402,14 @@
         <v>99</v>
       </c>
       <c r="C84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>102</v>
+      </c>
+      <c r="C85" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Listening mode bug fix.
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="103">
   <si>
     <t>Todos</t>
   </si>
@@ -40,12 +40,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Learn PCB Design</t>
-  </si>
-  <si>
-    <t>Read Practical Electronics</t>
-  </si>
-  <si>
     <t>Physical UI Design</t>
   </si>
   <si>
@@ -67,9 +61,6 @@
     <t>Antenna</t>
   </si>
   <si>
-    <t>Reset Circuit</t>
-  </si>
-  <si>
     <t>Only Forward if mutual buddies</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t>Status LEDs</t>
   </si>
   <si>
-    <t>Check Sparkfun guide</t>
-  </si>
-  <si>
     <t>Robustness against intercom restart</t>
   </si>
   <si>
@@ -344,6 +332,12 @@
   </si>
   <si>
     <t>Keep trying to connect to WiFi when in listening mode</t>
+  </si>
+  <si>
+    <t>Can't reproduce</t>
+  </si>
+  <si>
+    <t>Restore Default option in App</t>
   </si>
 </sst>
 </file>
@@ -680,10 +674,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,13 +699,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F1" s="2">
-        <v>43152</v>
+        <v>43174</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -719,58 +713,55 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -778,187 +769,187 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
       <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
       <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="C28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
       <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -966,7 +957,7 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -974,23 +965,23 @@
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -998,7 +989,7 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
@@ -1006,23 +997,26 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
@@ -1030,248 +1024,251 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>12</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C53" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C65" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
@@ -1279,7 +1276,7 @@
         <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
@@ -1287,53 +1284,53 @@
         <v>81</v>
       </c>
       <c r="C70" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
+        <v>85</v>
+      </c>
+      <c r="C74" t="s">
+        <v>41</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C74" t="s">
-        <v>45</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
@@ -1341,10 +1338,7 @@
         <v>89</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
@@ -1352,47 +1346,47 @@
         <v>90</v>
       </c>
       <c r="C77" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C78" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C79" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C80" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C82" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.3">
@@ -1400,7 +1394,7 @@
         <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.3">
@@ -1408,31 +1402,15 @@
         <v>99</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>103</v>
-      </c>
-      <c r="C86" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
-        <v>104</v>
-      </c>
-      <c r="C87" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added server name to cloud api
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -676,8 +676,8 @@
   </sheetPr>
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1370,7 @@
         <v>93</v>
       </c>
       <c r="C80" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.3">
@@ -1402,7 +1402,7 @@
         <v>99</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Major rework in progress due to introduction of database
</commit_message>
<xml_diff>
--- a/doc/ToDos.xlsx
+++ b/doc/ToDos.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="104">
   <si>
     <t>Todos</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Restore Default option in App</t>
+  </si>
+  <si>
+    <t>static message buffers take up too much space</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,6 +1414,14 @@
       </c>
       <c r="C85" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>103</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>